<commit_message>
[DOC] Update BOM and IO-MAP with relays and RTC
</commit_message>
<xml_diff>
--- a/Docs/BOM-REVAr_v0.0.xlsx
+++ b/Docs/BOM-REVAr_v0.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>VENDOR</t>
   </si>
@@ -127,28 +127,76 @@
     <t>NXP</t>
   </si>
   <si>
-    <t>LCD Display</t>
-  </si>
-  <si>
-    <t>RTC Module for I2C bus</t>
-  </si>
-  <si>
-    <t>DS1307</t>
-  </si>
-  <si>
-    <t>SPI SD Card Module</t>
-  </si>
-  <si>
     <t>4MD36</t>
   </si>
   <si>
     <t>SENSORES</t>
   </si>
   <si>
-    <t>RELAY</t>
-  </si>
-  <si>
-    <t>TRANSISTOR</t>
+    <t>https://www.filipeflop.com/produto/modulo-serial-i2c-para-display-lcd-arduino/</t>
+  </si>
+  <si>
+    <t>4MD22</t>
+  </si>
+  <si>
+    <t>Display LCD 16×2 Backlight Verde</t>
+  </si>
+  <si>
+    <t>5LC11</t>
+  </si>
+  <si>
+    <t>HD44780</t>
+  </si>
+  <si>
+    <t>HITACHI</t>
+  </si>
+  <si>
+    <t>https://www.filipeflop.com/produto/display-lcd-16x2-backlight-verde/</t>
+  </si>
+  <si>
+    <t>Real Time Clock RTC DS3231</t>
+  </si>
+  <si>
+    <t>DS3231</t>
+  </si>
+  <si>
+    <t>4MD09</t>
+  </si>
+  <si>
+    <t>https://www.filipeflop.com/produto/real-time-clock-rtc-ds3231/</t>
+  </si>
+  <si>
+    <t>Módulo Cartão Micro SD</t>
+  </si>
+  <si>
+    <t>https://www.filipeflop.com/produto/modulo-cartao-micro-sd/</t>
+  </si>
+  <si>
+    <t>Cartão de Memória Classe 10 16GB MicroSd</t>
+  </si>
+  <si>
+    <t>SANDISK</t>
+  </si>
+  <si>
+    <t>DRA17</t>
+  </si>
+  <si>
+    <t>https://www.filipeflop.com/produto/cartao-de-memoria-classe-10-16gb-microsd-sandisk/</t>
+  </si>
+  <si>
+    <t>SDSDQUNS-016G</t>
+  </si>
+  <si>
+    <t>Módulo Relé 5V 2 Canais</t>
+  </si>
+  <si>
+    <t>SRD-05VDC-SL-C</t>
+  </si>
+  <si>
+    <t>4MD04</t>
+  </si>
+  <si>
+    <t>https://www.filipeflop.com/produto/modulo-rele-5v-2-canais/</t>
   </si>
 </sst>
 </file>
@@ -156,7 +204,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -221,10 +269,10 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
@@ -232,8 +280,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -247,9 +295,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="5"/>
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Moneda 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -268,9 +316,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +356,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -380,7 +428,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,15 +602,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
@@ -715,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H25" si="0">G4*F4</f>
+        <f t="shared" ref="H4:H26" si="0">G4*F4</f>
         <v>27.6</v>
       </c>
       <c r="I4" s="5">
@@ -783,87 +831,218 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5">
+        <v>9.9</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.9</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="K6" s="14">
         <v>1</v>
       </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
+      <c r="D8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
       <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="5">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="0"/>
+        <v>74.900000000000006</v>
+      </c>
       <c r="I10" s="5"/>
-      <c r="K10" s="14"/>
+      <c r="J10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="G11" s="9">
+        <v>3</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="0"/>
+        <v>41.7</v>
+      </c>
       <c r="I11" s="5"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="J11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
       <c r="H13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -937,6 +1116,12 @@
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -947,8 +1132,14 @@
     <hyperlink ref="J3" r:id="rId2" location="tab-description"/>
     <hyperlink ref="J4" r:id="rId3"/>
     <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DOC] Add new sensors
</commit_message>
<xml_diff>
--- a/Docs/BOM-REVAr_v0.0.xlsx
+++ b/Docs/BOM-REVAr_v0.0.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARDUINO VERSION" sheetId="1" r:id="rId1"/>
+    <sheet name="Mouser Electronics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="95">
   <si>
     <t>VENDOR</t>
   </si>
@@ -197,14 +198,117 @@
   </si>
   <si>
     <t>https://www.filipeflop.com/produto/modulo-rele-5v-2-canais/</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Variável</t>
+  </si>
+  <si>
+    <t>Fabricante</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t>PRINCÍPIO MEDIÇÃO</t>
+  </si>
+  <si>
+    <t>APLICAÇÃO</t>
+  </si>
+  <si>
+    <t>MiCS-6814</t>
+  </si>
+  <si>
+    <t>MOS</t>
+  </si>
+  <si>
+    <t>SGX SENSORTECH</t>
+  </si>
+  <si>
+    <t>https://br.mouser.com/ProductDetail/Amphenol-SGX-Sensortech/MICS-6814?qs=sGAEpiMZZMtWSrBd5SaE4KIbT1yLGXllBQqf0A%2fWr%2f4pt%2fJ%252bcbCruw%3d%3d</t>
+  </si>
+  <si>
+    <t>DETECÇÃO</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>0.05 - 10ppm</t>
+  </si>
+  <si>
+    <t>1 - 1000 ppm</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>10 - 500ppm</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>1 - 1000ppm</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>1 - 500ppm</t>
+  </si>
+  <si>
+    <t>MiCS-5524</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> indoor carbon monoxide and natural gas leakage detection; suitable also for indoor air quality monitoring; breath checker and early fire detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> automobile exhausts and for agricultural/industrial odors</t>
+  </si>
+  <si>
+    <t>https://br.mouser.com/ProductDetail/Amphenol-SGX-Sensortech/MICS-5524?qs=sGAEpiMZZMtWSrBd5SaE4KIbT1yLGXllm%2ffJg7vFWzNHm%2f3mKiwGmQ%3d%3d</t>
+  </si>
+  <si>
+    <t>HPM Series</t>
+  </si>
+  <si>
+    <t>PM2.5</t>
+  </si>
+  <si>
+    <t>PM10</t>
+  </si>
+  <si>
+    <t>Datasheets\AIR SENSORS\HONEYWELL\honeywell-hpm32322550b-1275408.pdf</t>
+  </si>
+  <si>
+    <t>Datasheets\AIR SENSORS\SGX\1084_Datasheet-MiCS-5524-rev-8-1144838.pdf</t>
+  </si>
+  <si>
+    <t>Datasheets\AIR SENSORS\SGX\1143_Datasheet-MiCS-6814-rev-8-1144828.pdf</t>
+  </si>
+  <si>
+    <t>0 µg/m3 - 1,000 µg/m3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -258,12 +362,129 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -275,7 +496,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -293,6 +514,103 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -604,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1142,4 +1460,262 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="43">
+        <v>17.14</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="42"/>
+    </row>
+    <row r="7" spans="1:9" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="46">
+        <v>14.66</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="20" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" s="20" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" s="20" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="H22" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F2:F10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="Datasheets\GAS SENSORS\SGX\1143_Datasheet-MiCS-6814-rev-8-1144828.pdf"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="H7:H10" r:id="rId3" display="Datasheets\AIR SENSORS\SGX\1084_Datasheet-MiCS-5524-rev-8-1144838.pdf"/>
+    <hyperlink ref="I7" r:id="rId4"/>
+    <hyperlink ref="H21:H22" r:id="rId5" display="Datasheets\AIR SENSORS\HONEYWELL\honeywell-hpm32322550b-1275408.pdf"/>
+    <hyperlink ref="H2:H6" r:id="rId6" display="Datasheets\AIR SENSORS\SGX\1143_Datasheet-MiCS-6814-rev-8-1144828.pdf"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DOC] Add New SGX Sensor
</commit_message>
<xml_diff>
--- a/Docs/BOM-REVAr_v0.0.xlsx
+++ b/Docs/BOM-REVAr_v0.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="ARDUINO VERSION" sheetId="1" r:id="rId1"/>
     <sheet name="Mouser Electronics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>VENDOR</t>
   </si>
@@ -300,17 +300,29 @@
   </si>
   <si>
     <t>0 µg/m3 - 1,000 µg/m3</t>
+  </si>
+  <si>
+    <t>MiCS-4514</t>
+  </si>
+  <si>
+    <t>automobile exhausts</t>
+  </si>
+  <si>
+    <t>https://br.mouser.com/ProductDetail/?qs=YCa%2fAAYMW0137ZWFFytKcQ%3d%3d</t>
+  </si>
+  <si>
+    <t>Datasheets\AIR SENSORS\SGX\0278_Datasheet-MiCS-4514-rev-16-1144833.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -474,35 +486,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -514,107 +513,137 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="5"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Moneda 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +705,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,10 +737,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -743,7 +771,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -919,14 +946,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -942,7 +969,7 @@
     <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -980,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1097,7 +1124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
@@ -1136,7 +1163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1211,7 +1238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1247,7 +1274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1277,7 +1304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="9" customFormat="1">
       <c r="A10" s="9" t="s">
         <v>52</v>
       </c>
@@ -1314,7 +1341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="9" customFormat="1">
       <c r="A11" s="9" t="s">
         <v>57</v>
       </c>
@@ -1351,13 +1378,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="9" customFormat="1">
       <c r="F12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1366,79 +1393,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="H14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="H15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="H16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8">
       <c r="H17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8">
       <c r="H18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8">
       <c r="H19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:8">
       <c r="H20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:8">
       <c r="H21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:8">
       <c r="H22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:8">
       <c r="H23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:8">
       <c r="H24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:8">
       <c r="H25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:8">
       <c r="H26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1463,14 +1490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
@@ -1482,7 +1509,7 @@
     <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1511,188 +1538,282 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" s="16" customFormat="1">
+      <c r="A2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="41">
         <v>17.14</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="1:9" s="16" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="31"/>
+      <c r="B3" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" s="16" customFormat="1">
+      <c r="A4" s="31"/>
+      <c r="B4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="28" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" s="16" customFormat="1">
+      <c r="A5" s="31"/>
+      <c r="B5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="41"/>
-    </row>
-    <row r="6" spans="1:9" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A6" s="31"/>
+      <c r="B6" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="42"/>
-    </row>
-    <row r="7" spans="1:9" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" s="16" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A7" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="36" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="46">
+      <c r="F7" s="35"/>
+      <c r="G7" s="36">
         <v>14.66</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="38" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="20" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+    <row r="8" spans="1:9" s="16" customFormat="1" ht="33" customHeight="1">
+      <c r="A8" s="31"/>
+      <c r="B8" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" s="20" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="28" t="s">
+      <c r="D8" s="35"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" s="16" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:9" s="20" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" s="16" customFormat="1" ht="33" customHeight="1" thickBot="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="35"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1">
+      <c r="A11" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="51">
+        <v>15.98</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="17" customFormat="1">
+      <c r="A12" s="31"/>
+      <c r="B12" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="53"/>
+    </row>
+    <row r="13" spans="1:9" s="17" customFormat="1">
+      <c r="A13" s="31"/>
+      <c r="B13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="53"/>
+    </row>
+    <row r="14" spans="1:9" s="17" customFormat="1">
+      <c r="A14" s="31"/>
+      <c r="B14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="53"/>
+    </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="57"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="B22" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="26"/>
+      <c r="H22" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="21">
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="H11:H15"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I2:I6"/>
@@ -1707,6 +1828,8 @@
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="G2:G6"/>
     <mergeCell ref="H2:H6"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="D11:D15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="Datasheets\GAS SENSORS\SGX\1143_Datasheet-MiCS-6814-rev-8-1144828.pdf"/>
@@ -1715,6 +1838,8 @@
     <hyperlink ref="I7" r:id="rId4"/>
     <hyperlink ref="H21:H22" r:id="rId5" display="Datasheets\AIR SENSORS\HONEYWELL\honeywell-hpm32322550b-1275408.pdf"/>
     <hyperlink ref="H2:H6" r:id="rId6" display="Datasheets\AIR SENSORS\SGX\1143_Datasheet-MiCS-6814-rev-8-1144828.pdf"/>
+    <hyperlink ref="I11" r:id="rId7"/>
+    <hyperlink ref="H11:H15" r:id="rId8" display="Datasheets\AIR SENSORS\SGX\0278_Datasheet-MiCS-4514-rev-16-1144833.pdf"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>